<commit_message>
alteração na tabela de eventos
</commit_message>
<xml_diff>
--- a/Análise de Eventos/tabela_V2.xlsx
+++ b/Análise de Eventos/tabela_V2.xlsx
@@ -1,35 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1800794\Desktop\EngenhariaRequisitos\Tabela de eventos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\israe\EngenhariaRequisitos\Análise de Eventos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CFE113-7C9D-4E9F-89F6-C2232201347D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11535"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13290" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
+    <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
   <si>
     <t>Capacidades</t>
   </si>
@@ -113,13 +111,73 @@
   </si>
   <si>
     <t>x(4)</t>
+  </si>
+  <si>
+    <t>n°</t>
+  </si>
+  <si>
+    <t>Vender Roupa</t>
+  </si>
+  <si>
+    <t>Gerar Relatórios</t>
+  </si>
+  <si>
+    <t>Cadastro</t>
+  </si>
+  <si>
+    <t>Conciliar contas</t>
+  </si>
+  <si>
+    <t>Pagar contas</t>
+  </si>
+  <si>
+    <t>Gerar relaórios</t>
+  </si>
+  <si>
+    <t>Vender roupa</t>
+  </si>
+  <si>
+    <t>Cliente retira produtos</t>
+  </si>
+  <si>
+    <t>N°</t>
+  </si>
+  <si>
+    <t>Previsível</t>
+  </si>
+  <si>
+    <t>Não Previsível</t>
+  </si>
+  <si>
+    <t>Não Evento</t>
+  </si>
+  <si>
+    <t>Vendedor confirma pagamento</t>
+  </si>
+  <si>
+    <t>Final do dia: Loja gera relatório geral</t>
+  </si>
+  <si>
+    <t>Registrar Venda</t>
+  </si>
+  <si>
+    <t>Registrar Pagamento</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Cadastro de Roupa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vendedor </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,6 +194,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -286,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -356,6 +420,25 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -671,11 +754,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E6:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,4 +975,315 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0D7B4EF-616D-4FA8-8AFE-324AEAAB6BDA}">
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="25"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D1" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="27"/>
+      <c r="F1" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C29B2E8-5F72-43AC-ABE4-76F62761B02D}">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="31"/>
+    <col min="3" max="3" width="3.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="31" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="31">
+        <v>1</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="31">
+        <v>2</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="31">
+        <v>4</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="31">
+        <v>5</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="31">
+        <v>6</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="31">
+        <v>7</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="31">
+        <v>8</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="31">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="B2:B7"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>